<commit_message>
Update experiment E coli
</commit_message>
<xml_diff>
--- a/hacking_the_simplespectro/experiments/data_E_coli_experiment_5.xlsx
+++ b/hacking_the_simplespectro/experiments/data_E_coli_experiment_5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yann\simple-spectro\hacking_the_simplespectro\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB4217A-A993-4435-94F6-4BF9DDAB45EA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C2EFB7-181E-4A0E-B977-DB32BA19D4C3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{BE783F5F-AD5A-4260-A133-3E0A0A7545AA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="53">
   <si>
     <t>Experiment 4</t>
   </si>
@@ -120,12 +120,6 @@
     <t xml:space="preserve">Concentration uncertainty [mg/L] </t>
   </si>
   <si>
-    <t>Time [hh:mm]</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
     <t>inoculation</t>
   </si>
   <si>
@@ -154,13 +148,49 @@
   </si>
   <si>
     <t>"-0.00"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add. Meas. </t>
+  </si>
+  <si>
+    <t>s4</t>
+  </si>
+  <si>
+    <t>"0.00"</t>
+  </si>
+  <si>
+    <t>s5</t>
+  </si>
+  <si>
+    <t>s6</t>
+  </si>
+  <si>
+    <t>s7</t>
+  </si>
+  <si>
+    <t>s8</t>
+  </si>
+  <si>
+    <t>s9</t>
+  </si>
+  <si>
+    <t>Comment**</t>
+  </si>
+  <si>
+    <t>Time* [hh:mm]</t>
+  </si>
+  <si>
+    <t>*adding more bacterias at 14:39 since the growing phase seemed to have stopped</t>
+  </si>
+  <si>
+    <t>**</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +221,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +248,11 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -298,10 +348,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -319,7 +370,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -338,23 +388,31 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -368,6 +426,1000 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$6:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>h:mm</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.41041666666666665</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.42777777777777781</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.43263888888888885</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.43541666666666662</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44236111111111115</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46597222222222223</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47847222222222219</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.50277777777777777</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.50555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.55138888888888882</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.59513888888888888</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6118055555555556</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.6333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.67638888888888893</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.70208333333333339</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.72291666666666676</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.73333333333333339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$N$6:$N$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4371601994555212E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9483910933525241E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-3.0582483989209408E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5325522781921351E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5743138007389735E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1314590912880932E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.6181050324637177E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7330156547356666E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.0534247977652501E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4897789980160725E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.7185356300113871E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.4018302064021704E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.3527070947911202E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.9589615194645292E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.5118861433598766E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>6.9759999806401326E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9.1161487541632745E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-04F2-4171-ABD1-1DF5B97D5650}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="452912144"/>
+        <c:axId val="452911488"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="452912144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="h:mm" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="452911488"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="452911488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="452912144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>362067</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>84637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>310580</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>47565</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B5F716A-B1BD-4182-8028-D5BDD9719DFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -667,15 +1719,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C84FA36-92E7-4713-8B6D-40B3984C62FD}">
-  <dimension ref="A1:AG16"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="P5" sqref="P5:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14.33203125" bestFit="1" customWidth="1"/>
@@ -684,75 +1736,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AD1" s="16" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AD1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="AE1" s="16"/>
-      <c r="AF1" s="16"/>
-      <c r="AG1" s="16"/>
+      <c r="AE1" s="15"/>
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="15"/>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="21" t="s">
+      <c r="B2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
+      <c r="Z2" s="18"/>
       <c r="AD2" s="1" t="s">
         <v>4</v>
       </c>
@@ -767,36 +1819,36 @@
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
-      <c r="V3" s="12"/>
-      <c r="W3" s="12"/>
-      <c r="X3" s="12"/>
-      <c r="Y3" s="12"/>
-      <c r="Z3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
       <c r="AD3" s="3" t="s">
         <v>10</v>
       </c>
@@ -809,36 +1861,36 @@
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="17"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
-      <c r="Y4" s="12"/>
-      <c r="Z4" s="12"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
       <c r="AD4" s="3" t="s">
         <v>15</v>
       </c>
@@ -851,28 +1903,28 @@
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="11" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="26" t="s">
         <v>26</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -887,25 +1939,25 @@
       <c r="N5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="26" t="s">
         <v>26</v>
       </c>
       <c r="V5" s="1" t="s">
@@ -920,7 +1972,7 @@
       <c r="Y5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="26" t="s">
         <v>21</v>
       </c>
       <c r="AA5" s="5" t="s">
@@ -930,12 +1982,12 @@
         <v>28</v>
       </c>
       <c r="AC5" s="6"/>
-      <c r="AD5" s="13" t="s">
+      <c r="AD5" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
@@ -945,7 +1997,7 @@
         <v>0.41041666666666665</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="3">
@@ -975,7 +2027,10 @@
         <v>236.03679091757425</v>
       </c>
       <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
+      <c r="N6" s="3">
+        <f>LOG10(K$6/K6)</f>
+        <v>0</v>
+      </c>
       <c r="O6" s="7">
         <v>0.01</v>
       </c>
@@ -1024,7 +2079,7 @@
         <v>0.42777777777777781</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3">
@@ -1046,19 +2101,19 @@
         <v>37163</v>
       </c>
       <c r="K7" s="3">
-        <f t="shared" ref="K7:K16" si="0">AVERAGE(E7:J7)</f>
+        <f t="shared" ref="K7:K23" si="0">AVERAGE(E7:J7)</f>
         <v>37258.666666666664</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" ref="L7:L16" si="1">STDEV(E7:J7)</f>
+        <f t="shared" ref="L7:L23" si="1">STDEV(E7:J7)</f>
         <v>337.68663975151082</v>
       </c>
       <c r="M7" s="3">
         <v>0</v>
       </c>
       <c r="N7" s="3">
-        <f>LOG10(K$7/K7)</f>
-        <v>0</v>
+        <f>LOG10(K$6/K7)</f>
+        <v>1.4371601994555212E-3</v>
       </c>
       <c r="O7" s="7">
         <v>0</v>
@@ -1082,11 +2137,11 @@
         <v>-26</v>
       </c>
       <c r="V7" s="3">
-        <f t="shared" ref="V7:V16" si="2">AVERAGE(P7:U7)</f>
+        <f t="shared" ref="V7:V23" si="2">AVERAGE(P7:U7)</f>
         <v>76427</v>
       </c>
       <c r="W7" s="3">
-        <f t="shared" ref="W7:W16" si="3">STDEV(P7:U7)</f>
+        <f t="shared" ref="W7:W23" si="3">STDEV(P7:U7)</f>
         <v>56712.140033682379</v>
       </c>
       <c r="X7" s="3">
@@ -1097,11 +2152,11 @@
         <v>0</v>
       </c>
       <c r="Z7" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AA7" s="3">
         <f>Y7-N7</f>
-        <v>0</v>
+        <v>-1.4371601994555212E-3</v>
       </c>
       <c r="AB7" s="3">
         <f>SQRT(X7^2+M7^2)</f>
@@ -1119,7 +2174,7 @@
         <v>0.43263888888888885</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="3">
@@ -1153,8 +2208,8 @@
         <v>5.1711021066680627E-3</v>
       </c>
       <c r="N8" s="3">
-        <f t="shared" ref="N8:N16" si="4">LOG10(K$7/K8)</f>
-        <v>5.1123089389703928E-4</v>
+        <f t="shared" ref="N8:N23" si="4">LOG10(K$6/K8)</f>
+        <v>1.9483910933525241E-3</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="3">
@@ -1188,16 +2243,16 @@
         <v>0.62358435247356592</v>
       </c>
       <c r="Y8" s="3">
-        <f t="shared" ref="Y8:Y16" si="5">LOG10(V$7/V8)</f>
+        <f t="shared" ref="Y8:Y23" si="5">LOG10(V$7/V8)</f>
         <v>2.7632215793818857</v>
       </c>
       <c r="Z8" s="7"/>
       <c r="AA8" s="3">
-        <f t="shared" ref="AA8:AA16" si="6">Y8-N8</f>
-        <v>2.7627103484879889</v>
+        <f t="shared" ref="AA8:AA23" si="6">Y8-N8</f>
+        <v>2.7612731882885333</v>
       </c>
       <c r="AB8" s="3">
-        <f t="shared" ref="AB8:AB16" si="7">SQRT(X8^2+M8^2)</f>
+        <f t="shared" ref="AB8:AB23" si="7">SQRT(X8^2+M8^2)</f>
         <v>0.62360579290676421</v>
       </c>
       <c r="AD8" s="3">
@@ -1213,7 +2268,7 @@
         <v>0.43541666666666662</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="3">
@@ -1243,12 +2298,12 @@
         <v>165.27280478045986</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" ref="M9:M16" si="9">1/LN(10)*SQRT((L$7/K$7)^2 +(L9/K9)^2)</f>
+        <f t="shared" ref="M9:M23" si="9">1/LN(10)*SQRT((L$7/K$7)^2 +(L9/K9)^2)</f>
         <v>4.3789009675847005E-3</v>
       </c>
       <c r="N9" s="3">
         <f t="shared" si="4"/>
-        <v>-1.7429850393475793E-3</v>
+        <v>-3.0582483989209408E-4</v>
       </c>
       <c r="O9" s="7">
         <v>0</v>
@@ -1280,7 +2335,7 @@
         <v>28.44468315872054</v>
       </c>
       <c r="X9" s="3">
-        <f t="shared" ref="X9:X16" si="10">1/LN(10)*SQRT((W$7/V$7)^2 +(W9/V9)^2)</f>
+        <f t="shared" ref="X9:X23" si="10">1/LN(10)*SQRT((W$7/V$7)^2 +(W9/V9)^2)</f>
         <v>0.81510132908114918</v>
       </c>
       <c r="Y9" s="3" t="e">
@@ -1288,7 +2343,7 @@
         <v>#NUM!</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AA9" s="3" t="e">
         <f t="shared" si="6"/>
@@ -1311,7 +2366,7 @@
         <v>0.44236111111111115</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="3">
@@ -1346,7 +2401,7 @@
       </c>
       <c r="N10" s="3">
         <f t="shared" si="4"/>
-        <v>2.0953920787365973E-3</v>
+        <v>3.5325522781921351E-3</v>
       </c>
       <c r="O10" s="7">
         <v>0</v>
@@ -1409,7 +2464,7 @@
         <v>0.46597222222222223</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="3">
@@ -1444,7 +2499,7 @@
       </c>
       <c r="N11" s="3">
         <f t="shared" si="4"/>
-        <v>1.4305977807934222E-2</v>
+        <v>1.5743138007389735E-2</v>
       </c>
       <c r="O11" s="7">
         <v>0</v>
@@ -1484,11 +2539,11 @@
         <v>3.8353232601787357</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AA11" s="3">
         <f t="shared" si="6"/>
-        <v>3.8210172823708013</v>
+        <v>3.8195801221713461</v>
       </c>
       <c r="AB11" s="3">
         <f t="shared" si="7"/>
@@ -1507,7 +2562,7 @@
         <v>0.47847222222222219</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="7"/>
       <c r="E12" s="3">
@@ -1542,7 +2597,7 @@
       </c>
       <c r="N12" s="3">
         <f t="shared" si="4"/>
-        <v>9.8774307134254433E-3</v>
+        <v>1.1314590912880932E-2</v>
       </c>
       <c r="O12" s="7">
         <v>0.01</v>
@@ -1582,11 +2637,11 @@
         <v>3.9290043030565935</v>
       </c>
       <c r="Z12" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="AA12" s="3">
         <f t="shared" si="6"/>
-        <v>3.9191268723431683</v>
+        <v>3.9176897121437126</v>
       </c>
       <c r="AB12" s="3">
         <f t="shared" si="7"/>
@@ -1605,7 +2660,7 @@
         <v>0.50277777777777777</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="3">
@@ -1640,7 +2695,7 @@
       </c>
       <c r="N13" s="3">
         <f t="shared" si="4"/>
-        <v>1.4743890125181736E-2</v>
+        <v>1.6181050324637177E-2</v>
       </c>
       <c r="O13" s="7">
         <v>0</v>
@@ -1680,7 +2735,7 @@
         <v>#NUM!</v>
       </c>
       <c r="Z13" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AA13" s="3" t="e">
         <f t="shared" si="6"/>
@@ -1703,7 +2758,7 @@
         <v>0.50555555555555554</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="3">
@@ -1738,10 +2793,10 @@
       </c>
       <c r="N14" s="3">
         <f t="shared" si="4"/>
-        <v>1.5892996347901187E-2</v>
+        <v>1.7330156547356666E-2</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="P14" s="3">
         <v>12</v>
@@ -1778,7 +2833,7 @@
         <v>#NUM!</v>
       </c>
       <c r="Z14" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AA14" s="3" t="e">
         <f t="shared" si="6"/>
@@ -1797,132 +2852,857 @@
       <c r="A15" s="3">
         <v>9</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="10">
+        <v>0.55138888888888882</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="D15" s="7"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3" t="e">
+      <c r="E15" s="3">
+        <v>36427</v>
+      </c>
+      <c r="F15" s="3">
+        <v>36504</v>
+      </c>
+      <c r="G15" s="3">
+        <v>36462</v>
+      </c>
+      <c r="H15" s="3">
+        <v>36403</v>
+      </c>
+      <c r="I15" s="3">
+        <v>36570</v>
+      </c>
+      <c r="J15" s="3">
+        <v>36552</v>
+      </c>
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L15" s="3" t="e">
+        <v>36486.333333333336</v>
+      </c>
+      <c r="L15" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M15" s="3" t="e">
+        <v>67.351812645738548</v>
+      </c>
+      <c r="M15" s="3">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N15" s="3" t="e">
+        <v>4.0169541115198529E-3</v>
+      </c>
+      <c r="N15" s="3">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O15" s="7"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3"/>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3" t="e">
+        <v>1.0534247977652501E-2</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P15" s="3">
+        <v>-6</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>-18</v>
+      </c>
+      <c r="R15" s="3">
+        <v>-6</v>
+      </c>
+      <c r="S15" s="3">
+        <v>-4</v>
+      </c>
+      <c r="T15" s="3">
+        <v>27</v>
+      </c>
+      <c r="U15" s="3">
+        <v>-33</v>
+      </c>
+      <c r="V15" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W15" s="3" t="e">
+        <v>-6.666666666666667</v>
+      </c>
+      <c r="W15" s="3">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X15" s="3" t="e">
+        <v>19.815818596935799</v>
+      </c>
+      <c r="X15" s="3">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
+        <v>1.3305033865200091</v>
       </c>
       <c r="Y15" s="3" t="e">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z15" s="7"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="AA15" s="3" t="e">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB15" s="3" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="AB15" s="3">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD15" s="3" t="e">
+        <v>1.3305094503465758</v>
+      </c>
+      <c r="AD15" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>103557.27808368189</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>10</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
+      <c r="B16" s="10">
+        <v>0.59513888888888888</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="D16" s="7"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3" t="e">
+      <c r="E16" s="3">
+        <v>36676</v>
+      </c>
+      <c r="F16" s="3">
+        <v>36530</v>
+      </c>
+      <c r="G16" s="3">
+        <v>36685</v>
+      </c>
+      <c r="H16" s="3">
+        <v>36739</v>
+      </c>
+      <c r="I16" s="3">
+        <v>36704</v>
+      </c>
+      <c r="J16" s="3">
+        <v>36617</v>
+      </c>
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L16" s="3" t="e">
+        <v>36658.5</v>
+      </c>
+      <c r="L16" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M16" s="3" t="e">
+        <v>74.556689840684314</v>
+      </c>
+      <c r="M16" s="3">
         <f t="shared" si="9"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N16" s="3" t="e">
+        <v>4.0340300473703647E-3</v>
+      </c>
+      <c r="N16" s="3">
         <f t="shared" si="4"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="O16" s="7"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
-      <c r="R16" s="3"/>
-      <c r="S16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3" t="e">
+        <v>8.4897789980160725E-3</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P16" s="3">
+        <v>26</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>32</v>
+      </c>
+      <c r="R16" s="3">
+        <v>-21</v>
+      </c>
+      <c r="S16" s="3">
+        <v>-7</v>
+      </c>
+      <c r="T16" s="3">
+        <v>14</v>
+      </c>
+      <c r="U16" s="3">
+        <v>-28</v>
+      </c>
+      <c r="V16" s="3">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W16" s="3" t="e">
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="W16" s="3">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="X16" s="3" t="e">
+        <v>25.009331591761239</v>
+      </c>
+      <c r="X16" s="3">
         <f t="shared" si="10"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y16" s="3" t="e">
+        <v>4.0857597205074807</v>
+      </c>
+      <c r="Y16" s="3">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="3" t="e">
+        <v>4.4572780802236371</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA16" s="3">
         <f t="shared" si="6"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AB16" s="3" t="e">
+        <v>4.4487883012256209</v>
+      </c>
+      <c r="AB16" s="3">
         <f t="shared" si="7"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="AD16" s="3" t="e">
+        <v>4.0857617119846568</v>
+      </c>
+      <c r="AD16" s="3">
         <f t="shared" si="8"/>
-        <v>#DIV/0!</v>
+        <v>95028.959538275376</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>11</v>
+      </c>
+      <c r="B17" s="19">
+        <v>0.6118055555555556</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="20">
+        <v>36898</v>
+      </c>
+      <c r="F17" s="20">
+        <v>36854</v>
+      </c>
+      <c r="G17" s="20">
+        <v>36771</v>
+      </c>
+      <c r="H17" s="20">
+        <v>36965</v>
+      </c>
+      <c r="I17" s="20">
+        <v>36893</v>
+      </c>
+      <c r="J17" s="20">
+        <v>36978</v>
+      </c>
+      <c r="K17" s="20">
+        <f t="shared" si="0"/>
+        <v>36893.166666666664</v>
+      </c>
+      <c r="L17" s="20">
+        <f t="shared" si="1"/>
+        <v>75.945814016749253</v>
+      </c>
+      <c r="M17" s="20">
+        <f t="shared" si="9"/>
+        <v>4.0363939249681569E-3</v>
+      </c>
+      <c r="N17" s="3">
+        <f t="shared" si="4"/>
+        <v>5.7185356300113871E-3</v>
+      </c>
+      <c r="O17" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P17" s="20">
+        <v>-28</v>
+      </c>
+      <c r="Q17" s="20">
+        <v>3</v>
+      </c>
+      <c r="R17" s="20">
+        <v>-37</v>
+      </c>
+      <c r="S17" s="20">
+        <v>50</v>
+      </c>
+      <c r="T17" s="20">
+        <v>-36</v>
+      </c>
+      <c r="U17" s="20">
+        <v>1</v>
+      </c>
+      <c r="V17" s="20">
+        <f t="shared" si="2"/>
+        <v>-7.833333333333333</v>
+      </c>
+      <c r="W17" s="20">
+        <f t="shared" si="3"/>
+        <v>33.438999187575376</v>
+      </c>
+      <c r="X17" s="20">
+        <f t="shared" si="10"/>
+        <v>1.8817210328384575</v>
+      </c>
+      <c r="Y17" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z17" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA17" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB17" s="20">
+        <f t="shared" si="7"/>
+        <v>1.881725361975692</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>12</v>
+      </c>
+      <c r="B18" s="19">
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="C18" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="20">
+        <v>36881</v>
+      </c>
+      <c r="F18" s="20">
+        <v>36825</v>
+      </c>
+      <c r="G18" s="20">
+        <v>36812</v>
+      </c>
+      <c r="H18" s="20">
+        <v>36739</v>
+      </c>
+      <c r="I18" s="20">
+        <v>36832</v>
+      </c>
+      <c r="J18" s="20">
+        <v>36922</v>
+      </c>
+      <c r="K18" s="20">
+        <f t="shared" si="0"/>
+        <v>36835.166666666664</v>
+      </c>
+      <c r="L18" s="20">
+        <f t="shared" si="1"/>
+        <v>62.5121321558197</v>
+      </c>
+      <c r="M18" s="20">
+        <f t="shared" si="9"/>
+        <v>4.0045521455240761E-3</v>
+      </c>
+      <c r="N18" s="3">
+        <f t="shared" si="4"/>
+        <v>6.4018302064021704E-3</v>
+      </c>
+      <c r="O18" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P18" s="20">
+        <v>19</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>36</v>
+      </c>
+      <c r="R18" s="20">
+        <v>33</v>
+      </c>
+      <c r="S18" s="20">
+        <v>32</v>
+      </c>
+      <c r="T18" s="20">
+        <v>6</v>
+      </c>
+      <c r="U18" s="20">
+        <v>-25</v>
+      </c>
+      <c r="V18" s="20">
+        <f t="shared" si="2"/>
+        <v>16.833333333333332</v>
+      </c>
+      <c r="W18" s="20">
+        <f t="shared" si="3"/>
+        <v>23.370208956418569</v>
+      </c>
+      <c r="X18" s="20">
+        <f t="shared" si="10"/>
+        <v>0.68366370399440812</v>
+      </c>
+      <c r="Y18" s="20">
+        <f t="shared" si="5"/>
+        <v>3.6570766890969195</v>
+      </c>
+      <c r="Z18" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA18" s="20">
+        <f t="shared" si="6"/>
+        <v>3.6506748588905173</v>
+      </c>
+      <c r="AB18" s="20">
+        <f t="shared" si="7"/>
+        <v>0.68367543220247418</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>13</v>
+      </c>
+      <c r="B19" s="19">
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="C19" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="20">
+        <v>36848</v>
+      </c>
+      <c r="F19" s="20">
+        <v>36860</v>
+      </c>
+      <c r="G19" s="20">
+        <v>36853</v>
+      </c>
+      <c r="H19" s="20">
+        <v>36875</v>
+      </c>
+      <c r="I19" s="20">
+        <v>36795</v>
+      </c>
+      <c r="J19" s="20">
+        <v>36805</v>
+      </c>
+      <c r="K19" s="20">
+        <f t="shared" si="0"/>
+        <v>36839.333333333336</v>
+      </c>
+      <c r="L19" s="20">
+        <f t="shared" si="1"/>
+        <v>31.954133796219025</v>
+      </c>
+      <c r="M19" s="20">
+        <f t="shared" si="9"/>
+        <v>3.9541279832210202E-3</v>
+      </c>
+      <c r="N19" s="3">
+        <f t="shared" si="4"/>
+        <v>6.3527070947911202E-3</v>
+      </c>
+      <c r="O19" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P19" s="20">
+        <v>38</v>
+      </c>
+      <c r="Q19" s="20">
+        <v>13</v>
+      </c>
+      <c r="R19" s="20">
+        <v>-6</v>
+      </c>
+      <c r="S19" s="20">
+        <v>26</v>
+      </c>
+      <c r="T19" s="20">
+        <v>-45</v>
+      </c>
+      <c r="U19" s="20">
+        <v>-19</v>
+      </c>
+      <c r="V19" s="20">
+        <f t="shared" si="2"/>
+        <v>1.1666666666666667</v>
+      </c>
+      <c r="W19" s="20">
+        <f t="shared" si="3"/>
+        <v>30.668659355548403</v>
+      </c>
+      <c r="X19" s="20">
+        <f t="shared" si="10"/>
+        <v>11.421030008676873</v>
+      </c>
+      <c r="Y19" s="20">
+        <f t="shared" si="5"/>
+        <v>4.8163000228653052</v>
+      </c>
+      <c r="Z19" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA19" s="20">
+        <f t="shared" si="6"/>
+        <v>4.8099473157705139</v>
+      </c>
+      <c r="AB19" s="20">
+        <f t="shared" si="7"/>
+        <v>11.421030693165383</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>14</v>
+      </c>
+      <c r="B20" s="19">
+        <v>0.67638888888888893</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="20">
+        <v>36692</v>
+      </c>
+      <c r="F20" s="20">
+        <v>36658</v>
+      </c>
+      <c r="G20" s="20">
+        <v>36749</v>
+      </c>
+      <c r="H20" s="20">
+        <v>36643</v>
+      </c>
+      <c r="I20" s="20">
+        <v>36749</v>
+      </c>
+      <c r="J20" s="20">
+        <v>36729</v>
+      </c>
+      <c r="K20" s="20">
+        <f t="shared" si="0"/>
+        <v>36703.333333333336</v>
+      </c>
+      <c r="L20" s="20">
+        <f t="shared" si="1"/>
+        <v>46.159144994970035</v>
+      </c>
+      <c r="M20" s="20">
+        <f t="shared" si="9"/>
+        <v>3.9738565981745737E-3</v>
+      </c>
+      <c r="N20" s="3">
+        <f t="shared" si="4"/>
+        <v>7.9589615194645292E-3</v>
+      </c>
+      <c r="O20" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P20" s="20">
+        <v>-31</v>
+      </c>
+      <c r="Q20" s="20">
+        <v>-4</v>
+      </c>
+      <c r="R20" s="20">
+        <v>16</v>
+      </c>
+      <c r="S20" s="20">
+        <v>-22</v>
+      </c>
+      <c r="T20" s="20">
+        <v>-22</v>
+      </c>
+      <c r="U20" s="20">
+        <v>26</v>
+      </c>
+      <c r="V20" s="20">
+        <f t="shared" si="2"/>
+        <v>-6.166666666666667</v>
+      </c>
+      <c r="W20" s="20">
+        <f t="shared" si="3"/>
+        <v>23.016660632391194</v>
+      </c>
+      <c r="X20" s="20">
+        <f t="shared" si="10"/>
+        <v>1.6526986639087884</v>
+      </c>
+      <c r="Y20" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z20" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA20" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB20" s="20">
+        <f t="shared" si="7"/>
+        <v>1.6527034414020434</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>15</v>
+      </c>
+      <c r="B21" s="19">
+        <v>0.70208333333333339</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="20">
+        <v>36800</v>
+      </c>
+      <c r="F21" s="20">
+        <v>36848</v>
+      </c>
+      <c r="G21" s="20">
+        <v>36883</v>
+      </c>
+      <c r="H21" s="20">
+        <v>36847</v>
+      </c>
+      <c r="I21" s="20">
+        <v>36779</v>
+      </c>
+      <c r="J21" s="20">
+        <v>36798</v>
+      </c>
+      <c r="K21" s="20">
+        <f t="shared" si="0"/>
+        <v>36825.833333333336</v>
+      </c>
+      <c r="L21" s="20">
+        <f t="shared" si="1"/>
+        <v>39.605134347287184</v>
+      </c>
+      <c r="M21" s="20">
+        <f t="shared" si="9"/>
+        <v>3.9637580973373911E-3</v>
+      </c>
+      <c r="N21" s="3">
+        <f t="shared" si="4"/>
+        <v>6.5118861433598766E-3</v>
+      </c>
+      <c r="O21" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="P21" s="20">
+        <v>-6</v>
+      </c>
+      <c r="Q21" s="20">
+        <v>30</v>
+      </c>
+      <c r="R21" s="20">
+        <v>-24</v>
+      </c>
+      <c r="S21" s="20">
+        <v>10</v>
+      </c>
+      <c r="T21" s="20">
+        <v>7</v>
+      </c>
+      <c r="U21" s="20">
+        <v>-20</v>
+      </c>
+      <c r="V21" s="20">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="W21" s="20">
+        <f t="shared" si="3"/>
+        <v>20.295319657497391</v>
+      </c>
+      <c r="X21" s="20">
+        <f t="shared" si="10"/>
+        <v>17.631236114203073</v>
+      </c>
+      <c r="Y21" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z21" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA21" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB21" s="20">
+        <f t="shared" si="7"/>
+        <v>17.631236559758278</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>16</v>
+      </c>
+      <c r="B22" s="19">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="20">
+        <v>36694</v>
+      </c>
+      <c r="F22" s="20">
+        <v>36695</v>
+      </c>
+      <c r="G22" s="20">
+        <v>36721</v>
+      </c>
+      <c r="H22" s="20">
+        <v>36866</v>
+      </c>
+      <c r="I22" s="20">
+        <v>36908</v>
+      </c>
+      <c r="J22" s="20">
+        <v>36835</v>
+      </c>
+      <c r="K22" s="20">
+        <f t="shared" si="0"/>
+        <v>36786.5</v>
+      </c>
+      <c r="L22" s="20">
+        <f t="shared" si="1"/>
+        <v>94.502380922387346</v>
+      </c>
+      <c r="M22" s="20">
+        <f t="shared" si="9"/>
+        <v>4.0912050094557093E-3</v>
+      </c>
+      <c r="N22" s="3">
+        <f t="shared" si="4"/>
+        <v>6.9759999806401326E-3</v>
+      </c>
+      <c r="O22" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P22" s="20">
+        <v>11</v>
+      </c>
+      <c r="Q22" s="20">
+        <v>4</v>
+      </c>
+      <c r="R22" s="20">
+        <v>20</v>
+      </c>
+      <c r="S22" s="20">
+        <v>-16</v>
+      </c>
+      <c r="T22" s="20">
+        <v>14</v>
+      </c>
+      <c r="U22" s="20">
+        <v>0</v>
+      </c>
+      <c r="V22" s="20">
+        <f t="shared" si="2"/>
+        <v>5.5</v>
+      </c>
+      <c r="W22" s="20">
+        <f t="shared" si="3"/>
+        <v>12.708265027138834</v>
+      </c>
+      <c r="X22" s="20">
+        <f t="shared" si="10"/>
+        <v>1.0539559535748435</v>
+      </c>
+      <c r="Y22" s="20">
+        <f t="shared" si="5"/>
+        <v>4.1428841230016751</v>
+      </c>
+      <c r="Z22" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA22" s="20">
+        <f t="shared" si="6"/>
+        <v>4.1359081230210348</v>
+      </c>
+      <c r="AB22" s="20">
+        <f t="shared" si="7"/>
+        <v>1.0539638940847487</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A23" s="20">
+        <v>17</v>
+      </c>
+      <c r="B23" s="19">
+        <v>0.73333333333333339</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="20">
+        <v>36528</v>
+      </c>
+      <c r="F23" s="20">
+        <v>36500</v>
+      </c>
+      <c r="G23" s="20">
+        <v>36709</v>
+      </c>
+      <c r="H23" s="20">
+        <v>36644</v>
+      </c>
+      <c r="I23" s="20">
+        <v>36686</v>
+      </c>
+      <c r="J23" s="20">
+        <v>36567</v>
+      </c>
+      <c r="K23" s="20">
+        <f t="shared" si="0"/>
+        <v>36605.666666666664</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" si="1"/>
+        <v>86.363572567759533</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="9"/>
+        <v>4.0673193809493136E-3</v>
+      </c>
+      <c r="N23" s="3">
+        <f t="shared" si="4"/>
+        <v>9.1161487541632745E-3</v>
+      </c>
+      <c r="O23" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="P23" s="20">
+        <v>-6</v>
+      </c>
+      <c r="Q23" s="20">
+        <v>-37</v>
+      </c>
+      <c r="R23" s="20">
+        <v>25</v>
+      </c>
+      <c r="S23" s="20">
+        <v>-10</v>
+      </c>
+      <c r="T23" s="20">
+        <v>3</v>
+      </c>
+      <c r="U23" s="20">
+        <v>9</v>
+      </c>
+      <c r="V23" s="20">
+        <f t="shared" si="2"/>
+        <v>-2.6666666666666665</v>
+      </c>
+      <c r="W23" s="20">
+        <f t="shared" si="3"/>
+        <v>20.867838092784474</v>
+      </c>
+      <c r="X23" s="20">
+        <f t="shared" si="10"/>
+        <v>3.4137902270339215</v>
+      </c>
+      <c r="Y23" s="20" t="e">
+        <f t="shared" si="5"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="Z23" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA23" s="20" t="e">
+        <f t="shared" si="6"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="AB23" s="20">
+        <f t="shared" si="7"/>
+        <v>3.4137926500124842</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1939,5 +3719,7 @@
     <mergeCell ref="C2:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>